<commit_message>
Update: integrate digital and analog
</commit_message>
<xml_diff>
--- a/ACS712_AmMeter_Block_Diagram.xlsx
+++ b/ACS712_AmMeter_Block_Diagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\nerdfloor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\nerdfloor\Documents\Develop\ACS712_AmMeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39769C8-D6DA-48C4-8091-5266267ED87D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C742F97-66E2-49D5-9BAE-619CFB939884}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="195" windowWidth="20610" windowHeight="14940" xr2:uid="{ACC2928B-AA62-467B-931D-1973710DA547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACC2928B-AA62-467B-931D-1973710DA547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>IN</t>
     <phoneticPr fontId="1"/>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2020.01.05</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>デジタル系</t>
     <rPh sb="4" eb="5">
       <t>ケイ</t>
@@ -110,6 +106,22 @@
     <rPh sb="0" eb="3">
       <t>デンゲンケイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2020.01.19</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -761,21 +773,21 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="楕円 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F22A66B0-3F69-40B6-B463-F13E2BC016FB}"/>
+        <xdr:cNvPr id="11" name="楕円 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34995DB-B6B9-4AF7-AEA1-0BC09E48D853}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -783,7 +795,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4400550" y="4400550"/>
+          <a:off x="4400550" y="5600700"/>
           <a:ext cx="400050" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -819,23 +831,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="楕円 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34995DB-B6B9-4AF7-AEA1-0BC09E48D853}"/>
+        <xdr:cNvPr id="12" name="楕円 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D82F25-549A-4DD1-A297-A8DC11B8F5E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +855,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4400550" y="5600700"/>
+          <a:off x="9001125" y="3200400"/>
           <a:ext cx="400050" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -879,76 +891,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="楕円 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D82F25-549A-4DD1-A297-A8DC11B8F5E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9001125" y="3200400"/>
-          <a:ext cx="400050" cy="400050"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
+      <xdr:col>54</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -963,8 +915,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9001125" y="4400550"/>
-          <a:ext cx="400050" cy="400050"/>
+          <a:off x="10929938" y="6274595"/>
+          <a:ext cx="404813" cy="404812"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1907,62 +1859,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="直線矢印コネクタ 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5A80358-7822-439D-AC3E-0EECD3D8CFC2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="6"/>
-          <a:endCxn id="13" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4800600" y="4600575"/>
-          <a:ext cx="7000875" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>164225</xdr:colOff>
       <xdr:row>27</xdr:row>
@@ -3352,59 +3248,6 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="172" name="直線矢印コネクタ 171">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBCEA3D4-CBA1-4F63-A6FA-37E4CBE39368}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2226469" y="6477000"/>
-          <a:ext cx="607219" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -3692,6 +3535,578 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>2384</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="正方形/長方形 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7862E54-FA22-4F4A-9713-5D491228CF82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11337134" y="4655345"/>
+          <a:ext cx="1414460" cy="3845718"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Load</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="楕円 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF8BCF0-64A1-4793-9F5E-6E6B8C6A31FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10929938" y="5060157"/>
+          <a:ext cx="404813" cy="404813"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="楕円 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A61B0172-C85E-4579-A2C1-E4E1B658782B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10929938" y="7489032"/>
+          <a:ext cx="404813" cy="404813"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>188120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>188120</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="直線矢印コネクタ 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BF63BE-A185-429F-AE64-91E64296AE18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10322719" y="5248276"/>
+          <a:ext cx="607219" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="直線矢印コネクタ 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D632C8A-35AC-4CDC-A64B-B9BF3587F13D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10322719" y="7691438"/>
+          <a:ext cx="607219" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="コネクタ: カギ線 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2472F79E-8526-4D11-9E53-E7A531B1A53A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2428875" y="6477000"/>
+          <a:ext cx="8501063" cy="2631281"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 96499"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>202405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>202405</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="コネクタ: カギ線 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C809CF-2671-4DE4-82E6-040C90026CAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1012032" y="7691437"/>
+          <a:ext cx="2631281" cy="202406"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 226"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>134937</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="二等辺三角形 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85799EDF-32CC-4FE7-9F9F-6A9AAAD26E58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3508374" y="2079626"/>
+          <a:ext cx="809625" cy="674688"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>DIV</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>134937</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="コネクタ: カギ線 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DDCCB43-EF33-482E-82BA-478DC6D03A91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="78" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3008311" y="1849438"/>
+          <a:ext cx="1012033" cy="123031"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直線矢印コネクタ 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6AD59C5-77A8-46A2-85B6-6590319E15C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="78" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4250531" y="2416971"/>
+          <a:ext cx="2024063" cy="11904"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3999,8 +4414,8 @@
   </sheetPr>
   <dimension ref="B2:BD40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:BH45"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:BM47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4012,17 +4427,17 @@
     </row>
     <row r="3" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="BD5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="BD6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4030,7 +4445,7 @@
         <v>8</v>
       </c>
       <c r="BD7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4041,7 +4456,7 @@
         <v>10</v>
       </c>
       <c r="BD8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4060,12 +4475,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J25" t="s">
         <v>3</v>
       </c>
@@ -4078,13 +4493,16 @@
       <c r="AX25" t="s">
         <v>3</v>
       </c>
+      <c r="BC25" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="27" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J28" t="s">
         <v>7</v>
       </c>
@@ -4095,34 +4513,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J31" t="s">
         <v>4</v>
       </c>
-      <c r="O31" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX31" t="s">
-        <v>4</v>
+      <c r="BC31" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="34" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J34" t="s">
         <v>7</v>
       </c>
-      <c r="O34" t="s">
-        <v>6</v>
-      </c>
-      <c r="AX34" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="36" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J37" t="s">
         <v>5</v>
       </c>
@@ -4135,13 +4544,16 @@
       <c r="AX37" t="s">
         <v>5</v>
       </c>
+      <c r="BC37" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="39" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="10:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="10:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J40" t="s">
         <v>7</v>
       </c>
@@ -4155,7 +4567,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="71" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>